<commit_message>
App: IAS preferits App: Finestra de localització
</commit_message>
<xml_diff>
--- a/documents/IAS_IMATGES.xlsx
+++ b/documents/IAS_IMATGES.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="475">
   <si>
     <t>FITXER</t>
   </si>
@@ -1349,9 +1349,6 @@
     <t>Common waxbill and coin</t>
   </si>
   <si>
-    <t>IAS_id</t>
-  </si>
-  <si>
     <t>IAS_scientificname</t>
   </si>
   <si>
@@ -1419,6 +1416,66 @@
   </si>
   <si>
     <t>IASid</t>
+  </si>
+  <si>
+    <t>1;"Agave americana"</t>
+  </si>
+  <si>
+    <t>2;"Ailanthus altissima"</t>
+  </si>
+  <si>
+    <t>3;"Carpobrotus spp."</t>
+  </si>
+  <si>
+    <t>4;"Cortaderia selloana"</t>
+  </si>
+  <si>
+    <t>5;"Cotoneaster horizontalis"</t>
+  </si>
+  <si>
+    <t>6;"Estrilda astrild"</t>
+  </si>
+  <si>
+    <t>7;"Dreissena polymorpha"</t>
+  </si>
+  <si>
+    <t>8;"Pomacea insularum"</t>
+  </si>
+  <si>
+    <t>9;"Psittacula eupatria"</t>
+  </si>
+  <si>
+    <t>10;"Heracleum mantegazzianum"</t>
+  </si>
+  <si>
+    <t>11;"Senecio angulatus"</t>
+  </si>
+  <si>
+    <t>12;"Myiopsitta monachus"</t>
+  </si>
+  <si>
+    <t>13;"Psittacula krameri"</t>
+  </si>
+  <si>
+    <t>14;"Myocastor coypus"</t>
+  </si>
+  <si>
+    <t>15;"Opuntia spp."</t>
+  </si>
+  <si>
+    <t>16;"Phytolacca americana"</t>
+  </si>
+  <si>
+    <t>17;"Neovison vison"</t>
+  </si>
+  <si>
+    <t>18;"Procyon lotor"</t>
+  </si>
+  <si>
+    <t>IAS_id_postgresql_BB</t>
+  </si>
+  <si>
+    <t>IAS_Id_postgresql_Isaac</t>
   </si>
 </sst>
 </file>
@@ -1840,8 +1897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1861,7 +1918,7 @@
         <v>160</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1890,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>133</v>
@@ -1914,7 +1971,7 @@
         <v>46</v>
       </c>
       <c r="J2" t="str">
-        <f>VLOOKUP(B2,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B2,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Agave americana</v>
       </c>
     </row>
@@ -1923,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>134</v>
@@ -1947,7 +2004,7 @@
         <v>46</v>
       </c>
       <c r="J3" t="str">
-        <f>VLOOKUP(B3,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B3,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Agave americana</v>
       </c>
     </row>
@@ -1956,7 +2013,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
@@ -1971,7 +2028,7 @@
         <v>163</v>
       </c>
       <c r="J4" t="str">
-        <f>VLOOKUP(B4,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B4,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Agave americana</v>
       </c>
     </row>
@@ -1980,7 +2037,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>136</v>
@@ -1995,7 +2052,7 @@
         <v>163</v>
       </c>
       <c r="J5" t="str">
-        <f>VLOOKUP(B5,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B5,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Agave americana</v>
       </c>
     </row>
@@ -2004,7 +2061,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>137</v>
@@ -2019,7 +2076,7 @@
         <v>163</v>
       </c>
       <c r="J6" t="str">
-        <f>VLOOKUP(B6,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B6,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Agave americana</v>
       </c>
     </row>
@@ -2028,7 +2085,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
         <v>138</v>
@@ -2052,7 +2109,7 @@
         <v>46</v>
       </c>
       <c r="J7" t="str">
-        <f>VLOOKUP(B7,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B7,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Ailanthus altissima</v>
       </c>
     </row>
@@ -2061,7 +2118,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>251</v>
@@ -2076,7 +2133,7 @@
         <v>163</v>
       </c>
       <c r="J8" t="str">
-        <f>VLOOKUP(B8,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B8,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Ailanthus altissima</v>
       </c>
     </row>
@@ -2085,7 +2142,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
         <v>252</v>
@@ -2100,7 +2157,7 @@
         <v>163</v>
       </c>
       <c r="J9" t="str">
-        <f>VLOOKUP(B9,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B9,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Ailanthus altissima</v>
       </c>
     </row>
@@ -2109,7 +2166,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>141</v>
@@ -2124,7 +2181,7 @@
         <v>163</v>
       </c>
       <c r="J10" t="str">
-        <f>VLOOKUP(B10,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B10,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Ailanthus altissima</v>
       </c>
     </row>
@@ -2133,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
         <v>89</v>
@@ -2157,7 +2214,7 @@
         <v>46</v>
       </c>
       <c r="J11" t="str">
-        <f>VLOOKUP(B11,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B11,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Estrilda astrild</v>
       </c>
     </row>
@@ -2166,7 +2223,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
         <v>107</v>
@@ -2190,7 +2247,7 @@
         <v>46</v>
       </c>
       <c r="J12" t="str">
-        <f>VLOOKUP(B12,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B12,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Estrilda astrild</v>
       </c>
     </row>
@@ -2199,7 +2256,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="12">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
         <v>121</v>
@@ -2223,7 +2280,7 @@
         <v>46</v>
       </c>
       <c r="J13" t="str">
-        <f>VLOOKUP(B13,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B13,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Estrilda astrild</v>
       </c>
     </row>
@@ -2232,7 +2289,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="12">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>142</v>
@@ -2256,7 +2313,7 @@
         <v>46</v>
       </c>
       <c r="J14" t="str">
-        <f>VLOOKUP(B14,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B14,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Carpobrotus spp.</v>
       </c>
     </row>
@@ -2265,7 +2322,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="12">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>143</v>
@@ -2289,7 +2346,7 @@
         <v>46</v>
       </c>
       <c r="J15" t="str">
-        <f>VLOOKUP(B15,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B15,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Carpobrotus spp.</v>
       </c>
     </row>
@@ -2298,7 +2355,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="12">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>144</v>
@@ -2322,7 +2379,7 @@
         <v>46</v>
       </c>
       <c r="J16" t="str">
-        <f>VLOOKUP(B16,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B16,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Carpobrotus spp.</v>
       </c>
     </row>
@@ -2331,7 +2388,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
         <v>150</v>
@@ -2346,7 +2403,7 @@
         <v>163</v>
       </c>
       <c r="J17" t="str">
-        <f>VLOOKUP(B17,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B17,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Cortaderia selloana</v>
       </c>
     </row>
@@ -2355,7 +2412,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>151</v>
@@ -2370,7 +2427,7 @@
         <v>163</v>
       </c>
       <c r="J18" t="str">
-        <f>VLOOKUP(B18,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B18,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Cortaderia selloana</v>
       </c>
     </row>
@@ -2379,7 +2436,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
         <v>260</v>
@@ -2403,7 +2460,7 @@
         <v>46</v>
       </c>
       <c r="J19" t="str">
-        <f>VLOOKUP(B19,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B19,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Cortaderia selloana</v>
       </c>
     </row>
@@ -2412,7 +2469,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>43</v>
@@ -2436,7 +2493,7 @@
         <v>46</v>
       </c>
       <c r="J20" t="str">
-        <f>VLOOKUP(B20,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B20,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2445,7 +2502,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
         <v>152</v>
@@ -2469,7 +2526,7 @@
         <v>46</v>
       </c>
       <c r="J21" t="str">
-        <f>VLOOKUP(B21,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B21,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2478,7 +2535,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
         <v>153</v>
@@ -2502,7 +2559,7 @@
         <v>46</v>
       </c>
       <c r="J22" t="str">
-        <f>VLOOKUP(B22,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B22,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2511,7 +2568,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>67</v>
@@ -2535,7 +2592,7 @@
         <v>46</v>
       </c>
       <c r="J23" t="str">
-        <f>VLOOKUP(B23,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B23,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2544,7 +2601,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C24" t="s">
         <v>154</v>
@@ -2568,7 +2625,7 @@
         <v>46</v>
       </c>
       <c r="J24" t="str">
-        <f>VLOOKUP(B24,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B24,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2577,7 +2634,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="12">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>155</v>
@@ -2601,7 +2658,7 @@
         <v>46</v>
       </c>
       <c r="J25" t="str">
-        <f>VLOOKUP(B25,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B25,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Rhynchophorus ferrugineus</v>
       </c>
     </row>
@@ -2610,7 +2667,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="12">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
         <v>146</v>
@@ -2625,7 +2682,7 @@
         <v>163</v>
       </c>
       <c r="J26" t="str">
-        <f>VLOOKUP(B26,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B26,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myiopsitta monachus</v>
       </c>
     </row>
@@ -2634,7 +2691,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="12">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
         <v>275</v>
@@ -2658,7 +2715,7 @@
         <v>46</v>
       </c>
       <c r="J27" t="str">
-        <f>VLOOKUP(B27,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B27,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myiopsitta monachus</v>
       </c>
     </row>
@@ -2667,7 +2724,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="12">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
         <v>280</v>
@@ -2691,7 +2748,7 @@
         <v>46</v>
       </c>
       <c r="J28" t="str">
-        <f>VLOOKUP(B28,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B28,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myiopsitta monachus</v>
       </c>
     </row>
@@ -2700,7 +2757,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
         <v>156</v>
@@ -2715,7 +2772,7 @@
         <v>163</v>
       </c>
       <c r="J29" t="str">
-        <f>VLOOKUP(B29,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B29,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Opuntia spp.</v>
       </c>
     </row>
@@ -2724,7 +2781,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="12">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
         <v>284</v>
@@ -2748,7 +2805,7 @@
         <v>46</v>
       </c>
       <c r="J30" t="str">
-        <f>VLOOKUP(B30,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B30,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Opuntia spp.</v>
       </c>
     </row>
@@ -2757,7 +2814,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="12">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
         <v>157</v>
@@ -2772,7 +2829,7 @@
         <v>163</v>
       </c>
       <c r="J31" t="str">
-        <f>VLOOKUP(B31,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B31,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Senecio angulatus</v>
       </c>
     </row>
@@ -2781,7 +2838,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="12">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
         <v>158</v>
@@ -2796,7 +2853,7 @@
         <v>163</v>
       </c>
       <c r="J32" t="str">
-        <f>VLOOKUP(B32,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B32,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Senecio angulatus</v>
       </c>
     </row>
@@ -2805,7 +2862,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="12">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
         <v>288</v>
@@ -2829,7 +2886,7 @@
         <v>46</v>
       </c>
       <c r="J33" t="str">
-        <f>VLOOKUP(B33,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B33,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Psittacula krameri</v>
       </c>
     </row>
@@ -2838,7 +2895,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="12">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
         <v>265</v>
@@ -2853,7 +2910,7 @@
         <v>163</v>
       </c>
       <c r="J34" t="str">
-        <f>VLOOKUP(B34,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B34,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Psittacula krameri</v>
       </c>
     </row>
@@ -2862,7 +2919,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="12">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
         <v>300</v>
@@ -2886,7 +2943,7 @@
         <v>46</v>
       </c>
       <c r="J35" t="str">
-        <f>VLOOKUP(B35,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B35,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Cotoneaster horizontalis</v>
       </c>
     </row>
@@ -2895,7 +2952,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="12">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
         <v>302</v>
@@ -2919,7 +2976,7 @@
         <v>46</v>
       </c>
       <c r="J36" t="str">
-        <f>VLOOKUP(B36,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B36,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Cotoneaster horizontalis</v>
       </c>
     </row>
@@ -2928,7 +2985,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
         <v>308</v>
@@ -2952,7 +3009,7 @@
         <v>46</v>
       </c>
       <c r="J37" t="str">
-        <f>VLOOKUP(B37,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B37,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Dreissena polymorpha</v>
       </c>
     </row>
@@ -2961,7 +3018,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
         <v>311</v>
@@ -2985,7 +3042,7 @@
         <v>46</v>
       </c>
       <c r="J38" t="str">
-        <f>VLOOKUP(B38,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B38,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Dreissena polymorpha</v>
       </c>
     </row>
@@ -2994,7 +3051,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" t="s">
         <v>316</v>
@@ -3018,7 +3075,7 @@
         <v>46</v>
       </c>
       <c r="J39" t="str">
-        <f>VLOOKUP(B39,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B39,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Dreissena polymorpha</v>
       </c>
     </row>
@@ -3027,7 +3084,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="12">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
         <v>327</v>
@@ -3046,7 +3103,7 @@
         <v>325</v>
       </c>
       <c r="J40" t="str">
-        <f>VLOOKUP(B40,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B40,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Pomacea insularum</v>
       </c>
     </row>
@@ -3055,7 +3112,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="12">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>326</v>
@@ -3074,7 +3131,7 @@
         <v>325</v>
       </c>
       <c r="J41" t="str">
-        <f>VLOOKUP(B41,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B41,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Pomacea insularum</v>
       </c>
     </row>
@@ -3083,7 +3140,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="12">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C42" t="s">
         <v>338</v>
@@ -3107,7 +3164,7 @@
         <v>46</v>
       </c>
       <c r="J42" t="str">
-        <f>VLOOKUP(B42,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B42,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Psittacula eupatria</v>
       </c>
     </row>
@@ -3116,7 +3173,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="12">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C43" t="s">
         <v>341</v>
@@ -3140,7 +3197,7 @@
         <v>46</v>
       </c>
       <c r="J43" t="str">
-        <f>VLOOKUP(B43,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B43,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Psittacula eupatria</v>
       </c>
     </row>
@@ -3149,7 +3206,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
         <v>348</v>
@@ -3173,7 +3230,7 @@
         <v>46</v>
       </c>
       <c r="J44" t="str">
-        <f>VLOOKUP(B44,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B44,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Heracleum mantegazzianum</v>
       </c>
     </row>
@@ -3182,7 +3239,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
         <v>352</v>
@@ -3206,7 +3263,7 @@
         <v>46</v>
       </c>
       <c r="J45" t="str">
-        <f>VLOOKUP(B45,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B45,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Heracleum mantegazzianum</v>
       </c>
     </row>
@@ -3215,7 +3272,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
         <v>355</v>
@@ -3239,7 +3296,7 @@
         <v>46</v>
       </c>
       <c r="J46" t="str">
-        <f>VLOOKUP(B46,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B46,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Heracleum mantegazzianum</v>
       </c>
     </row>
@@ -3248,7 +3305,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="12">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
         <v>358</v>
@@ -3272,7 +3329,7 @@
         <v>46</v>
       </c>
       <c r="J47" t="str">
-        <f>VLOOKUP(B47,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B47,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Heracleum mantegazzianum</v>
       </c>
     </row>
@@ -3281,7 +3338,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
         <v>366</v>
@@ -3305,7 +3362,7 @@
         <v>46</v>
       </c>
       <c r="J48" t="str">
-        <f>VLOOKUP(B48,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B48,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myocastor coypus</v>
       </c>
     </row>
@@ -3314,7 +3371,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C49" t="s">
         <v>375</v>
@@ -3338,7 +3395,7 @@
         <v>46</v>
       </c>
       <c r="J49" t="str">
-        <f>VLOOKUP(B49,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B49,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myocastor coypus</v>
       </c>
     </row>
@@ -3347,7 +3404,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
         <v>369</v>
@@ -3371,7 +3428,7 @@
         <v>46</v>
       </c>
       <c r="J50" t="str">
-        <f>VLOOKUP(B50,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B50,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Myocastor coypus</v>
       </c>
     </row>
@@ -3404,7 +3461,7 @@
         <v>46</v>
       </c>
       <c r="J51" t="str">
-        <f>VLOOKUP(B51,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B51,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Phytolacca americana</v>
       </c>
     </row>
@@ -3437,7 +3494,7 @@
         <v>46</v>
       </c>
       <c r="J52" t="str">
-        <f>VLOOKUP(B52,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B52,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Phytolacca americana</v>
       </c>
     </row>
@@ -3446,7 +3503,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>383</v>
@@ -3470,7 +3527,7 @@
         <v>46</v>
       </c>
       <c r="J53" t="str">
-        <f>VLOOKUP(B53,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B53,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Neovison vison</v>
       </c>
     </row>
@@ -3479,7 +3536,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>386</v>
@@ -3503,7 +3560,7 @@
         <v>46</v>
       </c>
       <c r="J54" t="str">
-        <f>VLOOKUP(B54,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B54,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Neovison vison</v>
       </c>
     </row>
@@ -3512,7 +3569,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="12">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>389</v>
@@ -3536,7 +3593,7 @@
         <v>46</v>
       </c>
       <c r="J55" t="str">
-        <f>VLOOKUP(B55,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B55,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Neovison vison</v>
       </c>
     </row>
@@ -3545,7 +3602,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>400</v>
@@ -3569,7 +3626,7 @@
         <v>46</v>
       </c>
       <c r="J56" t="str">
-        <f>VLOOKUP(B56,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B56,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Procyon lotor</v>
       </c>
     </row>
@@ -3578,7 +3635,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>392</v>
@@ -3602,7 +3659,7 @@
         <v>46</v>
       </c>
       <c r="J57" t="str">
-        <f>VLOOKUP(B57,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B57,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Procyon lotor</v>
       </c>
     </row>
@@ -3611,7 +3668,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="12">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>396</v>
@@ -3635,7 +3692,7 @@
         <v>46</v>
       </c>
       <c r="J58" t="str">
-        <f>VLOOKUP(B58,PostgresSQL_IAS!$A$2:$B$22,2,FALSE)</f>
+        <f>VLOOKUP(B58,PostgresSQL_IAS!$A$2:$C$22,3,FALSE)</f>
         <v>Procyon lotor</v>
       </c>
     </row>
@@ -8063,195 +8120,312 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="109" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="17" t="s">
+        <v>474</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>473</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>432</v>
       </c>
-      <c r="B1" s="17" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="8">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="8">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="8">
+      <c r="D4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>436</v>
+      </c>
+      <c r="D5" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>437</v>
+      </c>
+      <c r="D6" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>438</v>
+      </c>
+      <c r="D7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="8">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" s="8">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>442</v>
+      </c>
+      <c r="D11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="B12" s="8">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>443</v>
+      </c>
+      <c r="D12" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="8">
+      <c r="B13" s="8">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>444</v>
+      </c>
+      <c r="D13" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>17</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>445</v>
+      </c>
+      <c r="D14" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="8">
+      <c r="B15" s="8">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>446</v>
+      </c>
+      <c r="D15" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>447</v>
+      </c>
+      <c r="D16" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>448</v>
+      </c>
+      <c r="D17" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>449</v>
+      </c>
+      <c r="D18" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="8">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>450</v>
+      </c>
+      <c r="D19" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" s="8">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>451</v>
+      </c>
+      <c r="D20" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>452</v>
+      </c>
+      <c r="D21" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="8">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="8">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="8">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="8">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="8">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="8">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="8">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="8">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="8">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="8">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="8">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B22" s="8">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="8">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>454</v>
+      <c r="D22" t="s">
+        <v>462</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>